<commit_message>
Plots of mortality and morphological changes
End
</commit_message>
<xml_diff>
--- a/Teratogénesis_R.xlsx
+++ b/Teratogénesis_R.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Otros ordenadores\Mi portátil\Laptop Drive\Toxicología Acuática\Artículos\Evaluation of embryotoxicity\Resultados para artículo\Código Github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC38DE60-13A8-4AC5-ACD8-55E0F43FF2BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F6F1E2-FED2-4E13-824D-6F690214A621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="4" xr2:uid="{9263EA93-14D1-42F1-AA0F-2BC1A3ABBCD3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="7" xr2:uid="{9263EA93-14D1-42F1-AA0F-2BC1A3ABBCD3}"/>
   </bookViews>
   <sheets>
     <sheet name="GMI Sedimento" sheetId="2" r:id="rId1"/>
@@ -140,9 +140,6 @@
     <t>Blood circulation</t>
   </si>
   <si>
-    <t>Pigmentatio head-body</t>
-  </si>
-  <si>
     <t>Pigmentation tail</t>
   </si>
   <si>
@@ -162,6 +159,9 @@
   </si>
   <si>
     <t>Site</t>
+  </si>
+  <si>
+    <t>Pigmentation head-body</t>
   </si>
 </sst>
 </file>
@@ -1801,7 +1801,7 @@
                   <c:v>Blood circulation</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Pigmentatio head-body</c:v>
+                  <c:v>Pigmentation head-body</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Pigmentation tail</c:v>
@@ -1914,7 +1914,7 @@
                   <c:v>Blood circulation</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Pigmentatio head-body</c:v>
+                  <c:v>Pigmentation head-body</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Pigmentation tail</c:v>
@@ -2027,7 +2027,7 @@
                   <c:v>Blood circulation</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Pigmentatio head-body</c:v>
+                  <c:v>Pigmentation head-body</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Pigmentation tail</c:v>
@@ -2140,7 +2140,7 @@
                   <c:v>Blood circulation</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Pigmentatio head-body</c:v>
+                  <c:v>Pigmentation head-body</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Pigmentation tail</c:v>
@@ -2253,7 +2253,7 @@
                   <c:v>Blood circulation</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Pigmentatio head-body</c:v>
+                  <c:v>Pigmentation head-body</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Pigmentation tail</c:v>
@@ -12391,7 +12391,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -19781,8 +19781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C05A915-56E5-4ACA-B82B-A6CA9004FA0A}">
   <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T28" sqref="T28"/>
+    <sheetView topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19845,7 +19845,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2">
         <v>45</v>
@@ -19951,7 +19951,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -20163,7 +20163,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -20216,7 +20216,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -20269,7 +20269,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -20322,7 +20322,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -20375,7 +20375,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -20428,7 +20428,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13">
         <v>100</v>
@@ -20534,7 +20534,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15">
         <v>100</v>
@@ -20746,7 +20746,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -20799,7 +20799,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -20852,7 +20852,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -20905,7 +20905,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -20958,7 +20958,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -21011,7 +21011,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B24">
         <v>60</v>
@@ -21117,7 +21117,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26">
         <v>60</v>
@@ -21329,7 +21329,7 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B30">
         <v>60</v>
@@ -21382,7 +21382,7 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31">
         <v>60</v>
@@ -21435,7 +21435,7 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -21488,7 +21488,7 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -21541,7 +21541,7 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -21594,7 +21594,7 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35">
         <v>55</v>
@@ -21700,7 +21700,7 @@
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37">
         <v>55</v>
@@ -21912,7 +21912,7 @@
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B41">
         <v>50</v>
@@ -21965,7 +21965,7 @@
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B42">
         <v>55</v>
@@ -22018,7 +22018,7 @@
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B43">
         <v>55</v>
@@ -22071,7 +22071,7 @@
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B44">
         <v>55</v>
@@ -22124,7 +22124,7 @@
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B45">
         <v>5</v>
@@ -22177,7 +22177,7 @@
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B46">
         <v>55</v>
@@ -22283,7 +22283,7 @@
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B48">
         <v>55</v>
@@ -22495,7 +22495,7 @@
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B52">
         <v>50</v>
@@ -22548,7 +22548,7 @@
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B53">
         <v>55</v>
@@ -22601,7 +22601,7 @@
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B54">
         <v>55</v>
@@ -22654,7 +22654,7 @@
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B55">
         <v>55</v>
@@ -22707,7 +22707,7 @@
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B56">
         <v>35</v>
@@ -22777,7 +22777,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -23113,7 +23113,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -23440,7 +23440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{823C0202-E93D-492E-AB98-56531025B74C}">
   <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A56"/>
     </sheetView>
   </sheetViews>
@@ -23504,7 +23504,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2">
         <v>55</v>
@@ -23610,7 +23610,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -23822,7 +23822,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -23875,7 +23875,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -23928,7 +23928,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -23981,7 +23981,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -24034,7 +24034,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -24087,7 +24087,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13">
         <v>15</v>
@@ -24193,7 +24193,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15">
         <v>20</v>
@@ -24405,7 +24405,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -24458,7 +24458,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -24511,7 +24511,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -24564,7 +24564,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -24617,7 +24617,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -24670,7 +24670,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B24">
         <v>50</v>
@@ -24776,7 +24776,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26">
         <v>50</v>
@@ -24988,7 +24988,7 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B30">
         <v>50</v>
@@ -25041,7 +25041,7 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31">
         <v>50</v>
@@ -25094,7 +25094,7 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -25147,7 +25147,7 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -25200,7 +25200,7 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -25253,7 +25253,7 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35">
         <v>45</v>
@@ -25359,7 +25359,7 @@
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37">
         <v>50</v>
@@ -25571,7 +25571,7 @@
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B41">
         <v>45</v>
@@ -25624,7 +25624,7 @@
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B42">
         <v>50</v>
@@ -25677,7 +25677,7 @@
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B43">
         <v>50</v>
@@ -25730,7 +25730,7 @@
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B44">
         <v>50</v>
@@ -25783,7 +25783,7 @@
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B45">
         <v>15</v>
@@ -25836,7 +25836,7 @@
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B46">
         <v>45</v>
@@ -25942,7 +25942,7 @@
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B48">
         <v>50</v>
@@ -26154,7 +26154,7 @@
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B52">
         <v>50</v>
@@ -26207,7 +26207,7 @@
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B53">
         <v>50</v>
@@ -26260,7 +26260,7 @@
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B54">
         <v>50</v>
@@ -26313,7 +26313,7 @@
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B55">
         <v>50</v>
@@ -26366,7 +26366,7 @@
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B56">
         <v>45</v>
@@ -26434,7 +26434,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Error in database translocation
</commit_message>
<xml_diff>
--- a/Teratogénesis_R.xlsx
+++ b/Teratogénesis_R.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Otros ordenadores\Mi portátil\Laptop Drive\Toxicología Acuática\Artículos\Evaluation of embryotoxicity\Resultados para artículo\Código Github\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\Código GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F6F1E2-FED2-4E13-824D-6F690214A621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C4E1A7-08DB-4059-9F0A-FF7AB119CC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="7" xr2:uid="{9263EA93-14D1-42F1-AA0F-2BC1A3ABBCD3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="4" xr2:uid="{9263EA93-14D1-42F1-AA0F-2BC1A3ABBCD3}"/>
   </bookViews>
   <sheets>
     <sheet name="GMI Sedimento" sheetId="2" r:id="rId1"/>
@@ -19781,8 +19781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C05A915-56E5-4ACA-B82B-A6CA9004FA0A}">
   <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:A56"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18:J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20652,31 +20652,31 @@
         <v>65</v>
       </c>
       <c r="E17">
-        <v>20</v>
+        <v>75</v>
       </c>
       <c r="F17">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="G17">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="H17">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="I17">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="J17">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="K17">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="M17">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="N17">
         <v>85</v>
@@ -20705,22 +20705,22 @@
         <v>65</v>
       </c>
       <c r="E18">
-        <v>20</v>
+        <v>75</v>
       </c>
       <c r="F18">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="G18">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="H18">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="I18">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="J18">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="K18">
         <v>45</v>
@@ -23440,7 +23440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{823C0202-E93D-492E-AB98-56531025B74C}">
   <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A56"/>
     </sheetView>
   </sheetViews>

</xml_diff>